<commit_message>
remove kth with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148FEE44-0665-FF49-ACDF-C71C7DE2070F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D39755-A634-144A-AF52-3BE09CB0B8A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="460" windowWidth="26040" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="5980" yWindow="2940" windowWidth="24020" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -303,6 +303,32 @@
   </si>
   <si>
     <t>lc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定一个链表，删除链表的倒数第n个节点，并且返回链表的头结点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. 快指针fast先从solder向前走n步
+2. 判断fast为空，就停止；不为空就继续向下
+3. fast没有达到尾部，fast与slow指针同时向前走一 步，slow走第一步时是从solder走的
+4. fast到达链表尾部(非空节点)，slow就指向倒数第n个节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>快慢指针
+滑动窗口
+solder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(L)，L是窗口长度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(1)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -724,7 +750,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -785,8 +811,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="F3" s="2"/>
+    <row r="3" spans="1:7" ht="140">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
remove kth summary  with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D39755-A634-144A-AF52-3BE09CB0B8A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899C980A-A0CD-6D43-8867-C726ACD15087}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="2940" windowWidth="24020" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="1180" yWindow="1240" windowWidth="24020" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -310,14 +310,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">
-1. 快指针fast先从solder向前走n步
-2. 判断fast为空，就停止；不为空就继续向下
-3. fast没有达到尾部，fast与slow指针同时向前走一 步，slow走第一步时是从solder走的
-4. fast到达链表尾部(非空节点)，slow就指向倒数第n个节点</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>快慢指针
 滑动窗口
 solder</t>
@@ -329,6 +321,329 @@
   </si>
   <si>
     <t>O(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>快指针</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>fast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>先从</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>solder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>向前走</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">步
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>判断</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>fast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">为空，就停止，确保n是一个有效范围；不为空就继续向下执行程序
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>3. fast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>没有达到尾部，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>fast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>与</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>slow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>指针同时向前走一</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>步，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>slow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>走第一步时是从</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>solder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">走的
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>4. fast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>到达链表尾部</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非空节点</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>slow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>就指向倒数第</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个节点</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -417,21 +732,24 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -765,74 +1083,177 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="35" customHeight="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" ht="35" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="108">
-      <c r="A2" s="1">
+    <row r="2" spans="1:11" ht="108">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>23</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="140">
-      <c r="A3" s="1">
+    <row r="3" spans="1:11" ht="154">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
swap node sumamry  with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899C980A-A0CD-6D43-8867-C726ACD15087}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2872117-DC40-0B4B-A327-F7C59D86C280}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1240" windowWidth="24020" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="24020" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -644,6 +644,27 @@
       </rPr>
       <t>个节点</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 从solder=cur节点开始，查找需要交换的两个节点
+2. 两个节点有一个为空，就退出程序，返回solder.next
+3. 如果这两个节点全部不为空，交换两个节点，cur指针前进两步
+4. 进入步骤2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定一个链表，两两交换其中相邻的节点，并返回交换后的链表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>solder
+链表插入
+节点交换</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(N), N是元素个数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1068,7 +1089,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1164,14 +1185,28 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+    <row r="4" spans="1:11" ht="120">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>

</xml_diff>

<commit_message>
rotate  with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2872117-DC40-0B4B-A327-F7C59D86C280}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B673707-E9F1-2844-A1E8-C221CD59E31B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="24020" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="21640" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -299,10 +299,6 @@
       </rPr>
       <t>空间复杂度</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -665,6 +661,60 @@
   </si>
   <si>
     <t>O(N), N是元素个数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 先找出倒数第k个节点的前一个节点slow【快慢指针+sodler+滑动窗口】，将链表截断，再将两段按照题意合并【第一段的头节点是head，尾节点是slow；第二段的头节点是slow.next，尾节点是fast】
+2 保存slow.next节点
+ slow当尾节点
+4 fast节点指向头节点
+5 slow.nexta当作头节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>solder
+快慢指针
+节点增加/删除
+链表旋转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leetcode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">给定一个链表，旋转链表，将链表每个节点向右移动 k </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个位置，其中</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> k </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是非负数。</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -672,7 +722,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -728,6 +778,13 @@
       <color theme="1"/>
       <name val="微软雅黑"/>
       <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -1088,14 +1145,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="4.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" customWidth="1"/>
     <col min="3" max="3" width="36" style="1" customWidth="1"/>
     <col min="4" max="4" width="52.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.1640625" style="1" customWidth="1"/>
@@ -1109,7 +1166,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
@@ -1166,19 +1223,19 @@
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -1193,33 +1250,47 @@
         <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+    <row r="5" spans="1:11" ht="160">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>61</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>

</xml_diff>

<commit_message>
rotate comment  with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B673707-E9F1-2844-A1E8-C221CD59E31B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F92A321-534C-DA48-8822-4E538A128B95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="460" windowWidth="21640" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -1146,7 +1146,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>

</xml_diff>

<commit_message>
reverse  with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6E08EF-4B26-4041-AFD2-2A66AF990920}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5FACB8-48BE-EF42-9802-3ACD3CE1670A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24460" yWindow="1240" windowWidth="24640" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -173,6 +173,25 @@
 快慢指针
 节点增加/删除
 排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 三个指针，分别指向当前节点cur，前一个节点prev，下一个节点next
+2 当前节点不为空，就向下执行；为空，就结束循环，返回
+3 保存cur节点的下一个节点到next
+4 当前指针cur指向prev
+5 当前指针cur赋值给prev
+6 下一个节点next赋值给cur指针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>反转一个单链表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前后指针
+当前指针
+链表插入/删除</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -575,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -753,14 +772,28 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+    <row r="7" spans="1:11" ht="160">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>206</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>

</xml_diff>

<commit_message>
reverse 2  with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5FACB8-48BE-EF42-9802-3ACD3CE1670A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809068E2-EC5F-E845-BC11-526695B69CCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -176,22 +176,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>反转一个单链表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前后指针
+当前指针
+链表插入/删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1 三个指针，分别指向当前节点cur，前一个节点prev，下一个节点next
-2 当前节点不为空，就向下执行；为空，就结束循环，返回
+2 当前节点不为空，就向下执行；为空，就结束循 环，返回
 3 保存cur节点的下一个节点到next
 4 当前指针cur指向prev
 5 当前指针cur赋值给prev
 6 下一个节点next赋值给cur指针</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>反转一个单链表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>前后指针
-当前指针
-链表插入/删除</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -772,26 +772,26 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="160">
-      <c r="A7" s="2">
+    <row r="7" spans="1:11" ht="176">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="4">
         <v>206</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H7" s="2"/>

</xml_diff>

<commit_message>
reverse 2 comment  with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809068E2-EC5F-E845-BC11-526695B69CCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADF6C28-6AE9-0D4E-8500-C5E2C888D13D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-37640" yWindow="-10600" windowWidth="26120" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -194,12 +194,232 @@
 6 下一个节点next赋值给cur指针</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>反转从位置 m 到 n 的链表。请使用一趟扫描完成反转</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        0 solder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">节点
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">         1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>根据指定的位置，将指针</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>prev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">移动到目标节点的前一个节点
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">         2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>按照链表反转的流程进行反转，注意从第</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个位置到第</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">个位置
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">         3 https://leetcode-cn.com/problems/reverse-linked-list-ii/solution/ji-bai-liao-100de-javayong-hu-by-reedfan-6/
+         4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>目标链表反转完毕，开始做拼接：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>cur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是目标链表之后的第一个节点，应将</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>cur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>赋值给目标链表的第一个节点的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>next</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">；
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">         5 prev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的下一个节点是目标链表的最后一个节点</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前置节点
+前后指针
+链表插入/删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -236,6 +456,19 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="SimSun"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11.3"/>
+      <color rgb="FF808080"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -259,7 +492,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -277,6 +510,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,7 +831,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -799,14 +1035,28 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+    <row r="8" spans="1:11" ht="256">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>92</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>

</xml_diff>

<commit_message>
is palindrome with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADF6C28-6AE9-0D4E-8500-C5E2C888D13D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421615D5-FB4D-8F43-A7A9-C3C6760246F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37640" yWindow="-10600" windowWidth="26120" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -198,220 +198,18 @@
     <t>反转从位置 m 到 n 的链表。请使用一趟扫描完成反转</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">        0 solder</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">节点
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">         1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>根据指定的位置，将指针</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>prev</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">移动到目标节点的前一个节点
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">         2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>按照链表反转的流程进行反转，注意从第</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>m</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>个位置到第</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">个位置
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">         3 https://leetcode-cn.com/problems/reverse-linked-list-ii/solution/ji-bai-liao-100de-javayong-hu-by-reedfan-6/
-         4 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>目标链表反转完毕，开始做拼接：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>cur</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>是目标链表之后的第一个节点，应将</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>cur</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>赋值给目标链表的第一个节点的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>next</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">；
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">         5 prev</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>的下一个节点是目标链表的最后一个节点</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>前置节点
 前后指针
 链表插入/删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">        0 solder节点
+         1 根据指定的位置，将指针prev移动到目标节点的前一个节点
+         2 按照链表反转的流程进行反转，注意从第m个位置到第n个位置
+         3 https://leetcode-cn.com/problems/reverse-linked-list-ii/solution/ji-bai-liao-100de-javayong-hu-by-reedfan-6/
+         4 目标链表反转完毕，开始做拼接：cur是目标链表之后的第一个节点，应将cur赋值给目标链表的第一个节点的next；
+         5 prev的下一个节点是目标链表的最后一个节点</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -419,7 +217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -458,16 +256,10 @@
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="SimSun"/>
-      <family val="3"/>
+      <color rgb="FF808080"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11.3"/>
-      <color rgb="FF808080"/>
-      <name val="Monaco"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -511,7 +303,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -830,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1035,21 +827,21 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="256">
-      <c r="A8" s="2">
+    <row r="8" spans="1:11" ht="308">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="4">
         <v>92</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
reorder with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421615D5-FB4D-8F43-A7A9-C3C6760246F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC819748-D971-F141-96C3-A86CE31ED5BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37640" yWindow="-10600" windowWidth="26120" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>

</xml_diff>

<commit_message>
partition with algo design  with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC819748-D971-F141-96C3-A86CE31ED5BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2030255-E7CF-5141-B818-6A3742CB2A0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37640" yWindow="-10600" windowWidth="26120" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-80" yWindow="460" windowWidth="26120" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -195,9 +195,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>反转从位置 m 到 n 的链表。请使用一趟扫描完成反转</t>
-  </si>
-  <si>
     <t>前置节点
 前后指针
 链表插入/删除</t>
@@ -212,12 +209,89 @@
          5 prev的下一个节点是目标链表的最后一个节点</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>反转从位置 m 到 n 的链表。请使用一趟扫描完成反转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>给定一个链表和一个特定值</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF808080"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF808080"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>，对链表进行分隔，使得所有小于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF808080"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> x </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF808080"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>的节点都在大于或等于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF808080"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> x </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF808080"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>的节点之前</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>两个指针
+链表插入/删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 创建小指针min，大指针max
+2 小指针连接小于目标值的节点，大指针连接大于等于目标值的节点
+3大指针的next要赋值为null，例如1-4-3-2-5-2
+4 小指针的next指向大指针链表的头部
+5 返回小指针头部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -255,11 +329,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="12"/>
       <color rgb="FF808080"/>
-      <name val="微软雅黑"/>
+      <name val="Monaco"/>
       <family val="2"/>
-      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF808080"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -284,7 +363,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -302,9 +381,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -622,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -834,14 +910,14 @@
       <c r="B8" s="4">
         <v>92</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>9</v>
@@ -854,14 +930,28 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+    <row r="9" spans="1:11" ht="120">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>86</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>

</xml_diff>

<commit_message>
reorder and algo design with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2030255-E7CF-5141-B818-6A3742CB2A0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D8CF0F-A53B-EE49-9B00-41ADDB99B807}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="460" windowWidth="26120" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-80" yWindow="460" windowWidth="22640" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -284,6 +284,65 @@
 3大指针的next要赋值为null，例如1-4-3-2-5-2
 4 小指针的next指向大指针链表的头部
 5 返回小指针头部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定一个链表，判断链表中是否有环</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>快慢指针法
+1 快慢指针初始指向头节点
+2 快指针&amp;&amp;快指针的next不为空
+2 快指针一次走两步，慢指针一次走一步
+3 判断是否相等，如果相等代表有环，快慢指针相遇，返回结果，退出程序；否则没有环
+4 循环结束，没有找到相等的节点，就代表没有相交点，返回false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>快慢指针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1）没有环：快指针走到链表尾部，就退出循环，慢指针访问了链表一半的数据，快指针访问了所有的数据，O(n/2) + O(n)，时间复杂度是O(n)
+2）有环：慢指针进入环之前，走过的长度是M，快指针在环中迭代的元素个数是M，即非环长度是M。
+慢指针进入环之后，快慢指针经过多长时间会相遇（经过多少次迭代）：快慢指针的距离(最大是环的长度N)/快慢指针差即1，遍历迭代次数O(M + N), 即最大是O(链表长度)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定一个链表，返回链表开始入环的第一个节点。 如果链表无环，则返回 null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 快慢指针同时指向链表头节点
+2 快指针以及后续指针不为空
+3 快指针走两步，慢指针走一步
+3 快慢指针对应的节点是否相等，如果相等就说明有环，进一步验证环的入口（有环就一定有入口）
+，快节点从头开始走，慢节点继续前进，步长均为1，当slow==fast，说明入口到了
+4 如果没有找到或者快节点为空，就说明没有环，返回null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 计算链表的中间节点：
+     链表长度是奇数，slow是链表中间节点
+      链表长度是偶数，slow是链表中间位置偏右侧的节点
+2 链表的后半部分反转，得到反转后的链表头部
+3 链表前半部分与反转后的链表穿插串联节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">//给定一个单链表 L：L0→L1→…→Ln-1→Ln ， 
+//将其重新排列后变为： L0→Ln→L1→Ln-1→L2→Ln-2→… </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>快慢指针
+链表反转
+两个链表拼接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(M+N),M,N是两个链表的元素个数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -696,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -957,18 +1016,75 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+    <row r="10" spans="1:11" ht="260">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>141</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" ht="180">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>142</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="120">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>143</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
intersection and algo design with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D8CF0F-A53B-EE49-9B00-41ADDB99B807}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E1C429-AAF5-A849-BFB5-2F9B43528D46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-80" yWindow="460" windowWidth="22640" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -343,6 +343,24 @@
   </si>
   <si>
     <t>O(M+N),M,N是两个链表的元素个数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编写一个程序，找到两个单链表相交的起始节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 双指针分别指向两个链表的头节点
+2 判断两个节点是否相等，若不相等则两个指针向后迭代；
+         如果两个链表长度相等，且没有交点，两指针同时到达null，此时null==null为true
+         如果交点前的链表长度相等，且有交点，则一次遍历即可找到
+         如果交点前的链表长度不相等，且有交点，则指针curA到达链表A的尾部，就指向链表B的头部，同理对指针curB适用，直到找到交点
+3 若相等就返回</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">双指针
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -755,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1086,6 +1104,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="13" spans="1:11" ht="220">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>160</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
del given node and algo design with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E1C429-AAF5-A849-BFB5-2F9B43528D46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC7BECC-4566-6241-B130-0856BC6F6982}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-80" yWindow="460" windowWidth="22640" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -361,6 +361,23 @@
   <si>
     <t xml:space="preserve">双指针
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除链表中等于给定值 val 的所有节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 迭代链表，当前元素的next是否是null，为空就结束循环，不为空就向下执行
+2 当前指针cur的下一个元素值是否是目标值
+3 如果不是目标值，继续迭代
+4 如果是目标值，cur.next=cur.next.next
+5 继续1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单指针
+删除节点</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -773,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1127,6 +1144,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="14" spans="1:11" ht="120">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>203</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
palindrome and algo design with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC7BECC-4566-6241-B130-0856BC6F6982}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C79A84-0306-3C42-9379-5F29F365D436}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-80" yWindow="460" windowWidth="22640" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -378,6 +378,27 @@
   <si>
     <t>单指针
 删除节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请判断一个链表是否为回文链表。 
+例如：1-2-2-1，1-2-3-2-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 找到链表的中间节点
+         链表长度是奇数，slow是链表中间节点，1-2-2-1
+         链表长度是偶数，slow是链表中间位置偏右侧的节点，1-2-3-2-1
+2 反转链表的后半部分
+         1-2 2-1
+         1-2 ，1-2-3，最后一个元素是中间节点，不用比较
+ 两个链表逐个比较节点是否有相等</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>链表反转
+中间节点
+链表迭代</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -790,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1167,6 +1188,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="15" spans="1:11" ht="200">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>234</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
two sum and algo design with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07FFAAA-6F1B-864E-8886-964870FEA406}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B42A39-8ADA-3147-9FA7-4B6E622FA630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-80" yWindow="460" windowWidth="22640" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -414,6 +414,45 @@
   </si>
   <si>
     <t>删除节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定一个单链表，把所有的奇数节点和偶数节点分别排在一起。请注意，这里的奇数节点和偶数节点指的是节点编号的奇偶性，而不是节点的值的奇偶性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 初始化奇偶位置头指针【迭代期间不动】以及奇偶位置移动指针【负责迭代】
+2 奇指针指向偶指针的next节点
+3 奇指针向后迭代【偶指针之后的节点】
+4 偶指针指向奇指针之后的节点
+5 偶指针向后迭代【奇指针之后的节点】
+6 判断偶指针以及偶指针的next是否是null【注意】
+7 奇数个节点的链表，最后的状态是even_cur链表尾部的null；odd_cur指向最后一个节点
+7 偶数个节点的链表，最后的状态是even_cur链表最后一个节点；odd_cur指向链表倒数第二个节点
+8 奇链表尾部的next【odd_cur】指向偶链表的头部
+9 返回奇链表的头部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>链表添加
+保存节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给你两个 非空 链表来代表两个非负整数。数字最高位位于链表开始位置。它们的每个节点只存储一位数字。将这两数相加会返回一个新的链表。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 两个链表分别入栈，入栈完毕
+2 取出栈顶元素，相加，获取相加之和【一位数字】以及进位
+3 循环：根据创建节点tmp，solder指向tmp，下一个节点要添加到solder之后
+4 考虑最高位有进位的情况。例如9，9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>栈
+链表反转
+链表添加</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -826,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1249,6 +1288,52 @@
         <v>5</v>
       </c>
     </row>
+    <row r="17" spans="1:7" ht="260">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>328</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="120">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>445</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
remove node sum 0 comment  with linked list
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B42A39-8ADA-3147-9FA7-4B6E622FA630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B759D57A-E691-AF4E-8286-30D5D0E232DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="460" windowWidth="22640" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22640" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -453,6 +453,30 @@
     <t>栈
 链表反转
 链表添加</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>solder方便处理1-2--3
+1 使用map，key是当前节点以及之前节点的累加和，value是当前节点对象
+2 迭代节点，cur对应的节点和存在多次，说明这中间是有连续元素和为0的节点，即1-2-3-4,&lt;0,0&gt;&lt;1,1&gt;&lt;3,2&gt;&lt;6,3&gt;&lt;3,-3&gt;&lt;7,4&gt;
+3 找到这个节点cur1，将cur.next=cur1.next
+4 如果没有连续节点和是0，在map中也能找到一次累加和，执行cur.next=cur1.next，也是一样的，因为cur=cur1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给你一个链表的头节点 head，请你编写代码，反复删去链表中由 总和 值为 0 的连续节点组成的序列，直到不存在这样的序列为止</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>solder
+删除节点
+节点累加和
+哈希表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(K)
+K是链表节点个数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -865,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1334,6 +1358,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="19" spans="1:7" ht="200">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1171</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
single number  with hash
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B759D57A-E691-AF4E-8286-30D5D0E232DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AC0A16-7135-D84B-819A-242ADBC86361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22640" windowHeight="15000" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22640" windowHeight="15000" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
+    <sheet name="哈希" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="71">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -477,6 +478,23 @@
   <si>
     <t>O(K)
 K是链表节点个数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定一个非空整数数组，除了某个元素只出现一次以外，其余每个元素均出现两次。找出那个只出现了一次的元素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>异或</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>异或方案
+异或性质：
+1）一个数字和0异或【xor，^】，结果是其本身
+2）一个数字和其本身异或，结果是0
+3）异或满足交换律和结合律:a^b^b^c^a = (a^a)^(b^b)^c=0^0^c=0^c=c
+0逐个与数组中的每个数字异或操作，剩余的就是只出现一次的那个数字</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -891,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1385,4 +1403,79 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A17B2E-7C89-9142-AF64-850FAB88A98B}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="64.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="35" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" ht="198">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>136</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
repeat DNA design  with hash
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AC0A16-7135-D84B-819A-242ADBC86361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA74B95-E370-9845-99D4-D0D9C74F40AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22640" windowHeight="15000" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="76">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -495,6 +495,34 @@
 2）一个数字和其本身异或，结果是0
 3）异或满足交换律和结合律:a^b^b^c^a = (a^a)^(b^b)^c=0^0^c=0^c=c
 0逐个与数组中的每个数字异或操作，剩余的就是只出现一次的那个数字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有 DNA 都由一系列缩写为 A，C，G 和 T 的核苷酸组成，例如：“ACGAATTCCG”。在研究 DNA 时，识别 DNA 中的重复序列有时会对研究非常有帮助</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 窗口长度是10
+2 从原字符串0索引开始滑动窗口，落入窗口的子字符串是否在迭代集合中
+3 存在，说明这个子字符串出现了至少一次了，放入结果集合中
+4 不存在，说明这个子字符串只出现了一次，就将其放入迭代集合中
+4 迭代完整个原字符串【注意窗口位置】
+5 返回结果字符串，注意去重</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>集合去重
+滑动窗口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">窗口长度L，原字符串长度N，N-L+1个子字符串，每个子字符串长度是L。
+时间复杂度：O((N-L+1)L),题目已假定L=10，即时间复杂度是O(N)        </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>空间复杂度：集合保存这些子字符串，需要的空间是(N-L+1)L。
+O((N-L+1)L)，题目已假定L=10，即空间复杂度是O(N)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1407,10 +1435,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A17B2E-7C89-9142-AF64-850FAB88A98B}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1474,6 +1502,74 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:11" ht="220">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>187</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="21">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" ht="21">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" ht="21">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" ht="21">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" ht="21">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
happy number  with hash
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA74B95-E370-9845-99D4-D0D9C74F40AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BDC181-C9C3-D24C-9916-EE3ED32DE78A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22640" windowHeight="15000" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="180" yWindow="460" windowWidth="22640" windowHeight="15000" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="80">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -523,6 +523,30 @@
   <si>
     <t>空间复杂度：集合保存这些子字符串，需要的空间是(N-L+1)L。
 O((N-L+1)L)，题目已假定L=10，即空间复杂度是O(N)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">编写一个算法来判断一个数 n 是不是快乐数。 
+[快乐数」定义为：对于一个正整数，每一次将该数替换为它每个位置上的数字的平方和，然后重复这个过程直到这个数变为 1，也可能是 无限循环 但始终变不到 1。
+如果 可以变为 1，那么这个数就是快乐数。 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 这个数字是否在集合中出现过，出现过就false，没出现过就加入集合，继续1
+1 拆解一个整数，分别将各位相加
+2 判断这个数的各位平方和是否是1
+3 是1，就返回true
+4 不是1，将平方之和作为新的数字
+5 继续循环</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>集合
+整数拆解</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未知</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1437,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A17B2E-7C89-9142-AF64-850FAB88A98B}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1525,14 +1549,28 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="21">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+    <row r="4" spans="1:11" ht="220">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>202</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="21">
       <c r="A5" s="4"/>

</xml_diff>

<commit_message>
number frequency  with hash
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BDC181-C9C3-D24C-9916-EE3ED32DE78A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E776A9D-42D6-C64D-BBC4-40297DFA4818}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="460" windowWidth="22640" windowHeight="15000" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-22500" yWindow="-14280" windowWidth="22640" windowHeight="15000" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="85">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -547,6 +547,33 @@
   </si>
   <si>
     <t>未知</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">给定一个非空的整数数组，返回其中出现频率前 k 高的元素。 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 hashmap存储每个数字对应的出现次数
+2 创建小顶堆，小顶堆的长度是k，存放的顺序是比较这个数字出现的次数。
+3 先添加元素【add】，如果堆长度大于k，就移除堆头部元素即出现次数最小的元素【remove/poll】；长度小于k，就继续循环。
+4 所有数字添加完成，小顶堆也就创建完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小顶堆
+哈希表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(n)
+堆的长度是k，哈希表的长度是n，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(nlogk)
+n是数组长度
+k是堆的长度</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1462,7 +1489,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1572,14 +1599,28 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="21">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+    <row r="5" spans="1:11" ht="154">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>347</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="21">
       <c r="A6" s="4"/>

</xml_diff>

<commit_message>
first unique comment  with hash
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70B32B4-3204-C648-ABE8-83E6E58606B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE13132D-10A3-F34E-B64F-7F014E0BB98B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27380" yWindow="-13720" windowWidth="25720" windowHeight="16340" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="94">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -616,12 +616,31 @@
     <t>O(n)，其中一个数组要将其对应的次数存入哈希表，n是这个数组的元素个数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>给定一个字符串，找到它的第一个不重复的字符，并返回它的索引。如果不存在，则返回 -1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 使用哈希表存储每个字符在字符串中的出现次数
+2 遍历每个k-v，如果v是1，就取出相应的字符
+3 判断其在字符串中的位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哈希表
+字符出现次数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(N)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -683,6 +702,13 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -706,7 +732,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -727,6 +753,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1544,8 +1573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A17B2E-7C89-9142-AF64-850FAB88A98B}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1701,14 +1730,28 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="21">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+    <row r="7" spans="1:11" ht="66">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>387</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="21">
       <c r="A8" s="4"/>

</xml_diff>

<commit_message>
diff in 2 strings with hash
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE13132D-10A3-F34E-B64F-7F014E0BB98B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B45E1C-0347-8F4A-97B3-4F975C354777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="10320" yWindow="1960" windowWidth="26880" windowHeight="16340" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -633,6 +633,27 @@
   </si>
   <si>
     <t>O(N)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 使用哈希表存储小字符串各个字符的次数
+2 迭代大字符串
+3 如果这个字符在map中是null，说明此字符是新增加的。
+4 如果这个字符在map中是0，说明这个字符与之前的重复，也应该考虑，如s="a", t="aa"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">给定两个字符串 s 和 t，它们只包含小写字母。 
+ 字符串 t 由字符串 s 随机重排，然后在随机位置添加一个字母。 
+请找出在 t 中被添加的字母。 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(M+N),M,N是两个字符串的长度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(N),N是较短字符串的长度</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1573,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A17B2E-7C89-9142-AF64-850FAB88A98B}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1753,14 +1774,28 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="21">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+    <row r="8" spans="1:11" ht="110">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>389</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
reverse string with hash
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B45E1C-0347-8F4A-97B3-4F975C354777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43C0469-F9BD-1B41-8B52-165E6F9D18D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10320" yWindow="1960" windowWidth="26880" windowHeight="16340" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="101">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -654,6 +654,22 @@
   </si>
   <si>
     <t>O(N),N是较短字符串的长度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 使用hashMap存储每个字符出现的次数
+2 将hashmap中的元素存入大顶堆【按照出现次数排序】
+3 迭代大顶堆的元素，按照其在map中的出现次数，使用StringBuilder存储相应次数字符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哈希表
+字符出现次数
+大顶堆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">给定一个字符串，请将字符串里的字符按照出现的频率降序排列。 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1592,10 +1608,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A17B2E-7C89-9142-AF64-850FAB88A98B}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1796,6 +1812,33 @@
       <c r="G8" s="4" t="s">
         <v>97</v>
       </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" ht="88">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>451</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
line in keyboard  with hash
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43C0469-F9BD-1B41-8B52-165E6F9D18D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75CCC31-6E30-BD47-B7D8-6509FA6576D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="104">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -670,6 +670,21 @@
   </si>
   <si>
     <t xml:space="preserve">给定一个字符串，请将字符串里的字符按照出现的频率降序排列。 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(N*M), N是数组长度，M是字符串长度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">给定一个单词列表，只返回可以使用在键盘同一行的字母打印出来的单词。键盘如下图所示。 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 获取键盘中三行字符的位置，自己构建map
+2 解析字符串的字符，保留其位置，迭代下一个字符，并与prev比较，
+3 如果不相等就说明不相登，false
+4 如果相等就继续比较</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1608,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A17B2E-7C89-9142-AF64-850FAB88A98B}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1840,6 +1855,40 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
+    <row r="10" spans="1:11" ht="110">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>500</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" ht="21">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
top k 2  with hash
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75CCC31-6E30-BD47-B7D8-6509FA6576D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF4C14E-F5D6-8C43-B098-5DE93A408FB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-27200" yWindow="-10580" windowWidth="26880" windowHeight="15020" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="107">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -685,6 +685,26 @@
 2 解析字符串的字符，保留其位置，迭代下一个字符，并与prev比较，
 3 如果不相等就说明不相登，false
 4 如果相等就继续比较</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 使用map计算每个单词出现的次数
+2 使用小顶堆存储字符串，按照其在map出现的次数【如果次数相等，就使用字符串的比较大小功能】。
+3 小顶堆的长度限定在k【先增加然后删除堆顶元素，即可保证堆内是前k个大的字符串】
+ 4 迭代小顶堆，将元素插入链表中【每次插入0位置，既可保证了逆序输出】</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给一非空的单词列表，返回前 k 个出现次数最多的单词。 
+//
+// 返回的答案应该按单词出现频率由高到低排序。如果不同的单词有相同出现频率，按字母顺序排序。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哈希表
+字符出现次数
+小顶堆
+逆序输出小顶堆</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1625,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A17B2E-7C89-9142-AF64-850FAB88A98B}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1879,12 +1899,22 @@
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="21">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+    <row r="11" spans="1:11" ht="154">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>692</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>

</xml_diff>

<commit_message>
count character  with hash
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF4C14E-F5D6-8C43-B098-5DE93A408FB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE77F86-AB21-A846-B336-8FB6EF041DFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27200" yWindow="-10580" windowWidth="26880" windowHeight="15020" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="109">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -705,6 +705,22 @@
 字符出现次数
 小顶堆
 逆序输出小顶堆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 给定一个字符串b，里面包含多个字母
+2 构建map，存储b中的字符以及出现次数
+3 给定一个字符串数组arr，每个字符串a由字母组成
+4 字符串数组arr中的字符串a，是否由给定的字符串b中的字符组成？
+5 迭代字符串b中的字符，在map每出现一次，map中的value减少一次【map需要保存原始信息】
+6 如果这个字符串符合条件，就累加单词的长度之和</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">//给你一份『词汇表』（字符串数组） words 和一张『字母表』（字符串） chars。 
+// 假如你可以用 chars 中的『字母』（字符）拼写出 words 中的某个『单词』（字符串），那么我们就认为你掌握了这个单词。 
+// 注意：每次拼写（指拼写词汇表中的一个单词）时，chars 中的每个字母都只能用一次。 
+// 返回词汇表 words 中你掌握的所有单词的 长度之和。 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1643,10 +1659,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A17B2E-7C89-9142-AF64-850FAB88A98B}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1919,6 +1935,25 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
+    <row r="12" spans="1:11" ht="264">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1160</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
long sub str  with dp
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EC81DD-9E0F-3941-B579-9D44283B8C3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE173E6-03E9-134B-8137-090CC0DF5C33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" activeTab="2" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-35920" yWindow="-13680" windowWidth="26880" windowHeight="16340" activeTab="2" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="117">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -744,12 +744,38 @@
 dp[i] = i, i &lt; 2 &amp;&amp; i &gt; -1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve">给定一个无序的整数数组，找到其中最长上升子序列的长度。 
+示例: 
+输入: [10,9,2,5,3,7,101,18]
+输出: 4 
+解释: 最长的上升子序列是 [2,3,7,101]，它的长度是 4。 
+说明: 
+可能会有多种最长上升子序列的组合，你只需要输出对应的长度即可。 
+你算法的时间复杂度应该为 O(n2) 。 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 dp[i]代表以nums[i]结尾的子序列的最大长度
+2 dp[0]=1,以num[0]结尾的子序列即元素本身，最大长度是1
+3  例如：计算dp[5]，就需要计算dp[4]，即以4结尾的最大子序列长度
+4 dp中存储各个数字对应的最大递增序列长度，需要遍历数组，获取最大长度"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最长子序列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(n*n)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -818,13 +844,6 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
-    <font>
-      <i/>
-      <sz val="10.5"/>
-      <color rgb="FF629755"/>
-      <name val="Monaco"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -848,7 +867,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -872,9 +891,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1996,7 +2012,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2060,14 +2076,28 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="21">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+    <row r="3" spans="1:11" ht="242">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>300</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>111</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
sub str len comment  with dp
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE173E6-03E9-134B-8137-090CC0DF5C33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00406D3B-CC99-DD4B-A0DF-FBC421D880ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35920" yWindow="-13680" windowWidth="26880" windowHeight="16340" activeTab="2" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-29180" yWindow="1100" windowWidth="26880" windowHeight="16340" activeTab="2" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="120">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -768,6 +768,32 @@
   </si>
   <si>
     <t>O(n*n)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定一个未经排序的整数数组，找到最长且连续的的递增序列。 
+ 示例 1:
+输入: [1,3,5,4,7]
+输出: 3
+解释: 最长连续递增序列是 [1,3,5], 长度为3。
+尽管 [1,3,5,7] 也是升序的子序列, 但它不是连续的，因为5和7在原数组里被4隔开。 
+ 示例 2:
+输入: [2,2,2,2,2]
+输出: 1
+解释: 最长连续递增序列是 [2], 长度为1。
+ 注意：数组长度不会超过10000。
+ Related Topics 数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最长连续递增子序列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 dp[i]代表以nums[i]结尾的连续递增子序列的最大长度，状态方程：dp[i] = Math.max(dp[i], dp[i - 1] + 1);
+2 dp[0]=1,以num[0]结尾的子序列即元素本身，最大长度是1
+3  例如：计算dp[5]，就需要计算dp[4]，即以4结尾的最大子序列长度
+4 dp中存储各个数字对应的最大连续递增序列长度，需要遍历数组，获取最大长度</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2009,21 +2035,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D612D33-0305-F745-9965-094AE6CFAC6A}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="6.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="39.6640625" customWidth="1"/>
-    <col min="4" max="4" width="72.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" customWidth="1"/>
-    <col min="7" max="7" width="30.1640625" customWidth="1"/>
+    <col min="3" max="3" width="65.33203125" customWidth="1"/>
+    <col min="4" max="4" width="84.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="35" customHeight="1">
@@ -2099,6 +2125,29 @@
         <v>111</v>
       </c>
     </row>
+    <row r="4" spans="1:11" ht="374">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>674</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
roman to int  with math
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00406D3B-CC99-DD4B-A0DF-FBC421D880ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13517C7-BF04-FA4B-9BC3-03FCEDA8060C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29180" yWindow="1100" windowWidth="26880" windowHeight="16340" activeTab="2" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-38360" yWindow="460" windowWidth="26880" windowHeight="16340" activeTab="3" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
     <sheet name="哈希" sheetId="2" r:id="rId2"/>
     <sheet name="动态规划" sheetId="3" r:id="rId3"/>
+    <sheet name="数学" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="120">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2037,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D612D33-0305-F745-9965-094AE6CFAC6A}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2079,7 +2080,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="154">
+    <row r="2" spans="1:11" ht="132">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2102,7 +2103,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="242">
+    <row r="3" spans="1:11" ht="198">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2125,7 +2126,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="374">
+    <row r="4" spans="1:11" ht="308">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2145,6 +2146,73 @@
         <v>111</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E584FD4-BA79-F944-99BC-B54BFFE20F3C}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="65.5" customWidth="1"/>
+    <col min="4" max="4" width="58.83203125" customWidth="1"/>
+    <col min="5" max="5" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="20.5" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="35" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" ht="22">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
binary sum  improve with math
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E17A92-426D-0C47-BD31-76C3445F216D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E78BCE3-8B82-6242-A8CB-DF807C7CD911}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38360" yWindow="460" windowWidth="26880" windowHeight="16340" activeTab="3" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-66600" yWindow="-6040" windowWidth="26880" windowHeight="16340" activeTab="3" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="128">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -834,6 +834,51 @@
 3 如果匹配成功就累加对应的数字，并且指针向前移动2;如果两个字符串匹配不成功，就匹配一个
 4 匹配一个如果成功就累加；不成功就跳过。
 5 注意如果字符串没有对应的罗马字符，要如何处理？在for循环中设定i++,无论是否执行for中的条件，for循环都会继续前进</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>171
+#1290</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">N进制转换成十进制之和：
+         1 从左到右遍历每一位，即从高位累加，而非低位
+         2 累加和sum，sum = sum * N + val
+         3 原理介绍：
+              例如数字abc，十进制是a*100 + b * 10 + c
+              转换后变成： (a*10+b)*10+c
+              即可循环迭代每一位数字
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#171
+给定一个Excel表格中的列名称，返回其相应的列序号。 
+ 例如， 
+     A -&gt; 1
+    B -&gt; 2
+    C -&gt; 3
+    ...
+    Z -&gt; 26
+    AA -&gt; 27
+    AB -&gt; 28 
+    ...
+ 输入: "A"  输出: 1
+ 输入: "AB"   输出: 28
+ 输入: "ZY"  输出: 701 
+#1290
+给你一个单链表的引用结点 head。链表中每个结点的值不是 0 就 1。已知此链表是一个整数数字的二进制表示形式。 
+ 请你返回该链表所表示数字的 十进制值 。 
+ 输入：head = [1,0,1]
+输出：5
+解释：二进制数 (101) 转化为十进制数 (5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学
+进制转换
+累加</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2196,10 +2241,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E584FD4-BA79-F944-99BC-B54BFFE20F3C}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2244,7 +2289,9 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="4">
+        <v>168</v>
+      </c>
       <c r="C2" s="4" t="s">
         <v>122</v>
       </c>
@@ -2258,6 +2305,29 @@
         <v>120</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="409.6">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ugly number comment  with math
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E78BCE3-8B82-6242-A8CB-DF807C7CD911}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA244418-D193-FA47-8AF2-14EB87E512EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-66600" yWindow="-6040" windowWidth="26880" windowHeight="16340" activeTab="3" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-34380" yWindow="-13780" windowWidth="26880" windowHeight="16340" activeTab="3" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="131">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -879,6 +879,27 @@
     <t>数学
 进制转换
 累加</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">编写一个程序判断给定的数是否为丑数。 
+丑数就是只包含质因数 2, 3, 5 的正整数。 
+输入: 6
+输出: true
+解释: 6 = 2 × 3 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>循环取余数
+数学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 如果一个数是丑数，则uglyNumber = i*2 + j*3 + k*5, i,j,k属于[0,无穷大]
+2 先将此数循环除以2,最后得到的数不能整除2为止，进入3
+3 先将2中的数循环除以3,最后得到的数不能整除3为止，进入4
+4 先将4中的数循环除以4,最后得到的数不能整除5为止，进入5
+5 最后判断这个数字是否是1，如果是1，则是丑数，否则非丑数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2241,10 +2262,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E584FD4-BA79-F944-99BC-B54BFFE20F3C}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2331,6 +2352,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:11" ht="220">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>263</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sum of sqaure comment  with math
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA244418-D193-FA47-8AF2-14EB87E512EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEED474-9AD9-B442-A50F-2741AA0C1060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34380" yWindow="-13780" windowWidth="26880" windowHeight="16340" activeTab="3" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" activeTab="3" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="135">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -900,6 +900,29 @@
 3 先将2中的数循环除以3,最后得到的数不能整除3为止，进入4
 4 先将4中的数循环除以4,最后得到的数不能整除5为止，进入5
 5 最后判断这个数字是否是1，如果是1，则是丑数，否则非丑数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 存在两个整数a,b，例如-2，-1，-，1，2，3，4，5，他们的平方之和等于指定的数c
+2 a*a,b*b的值分别小于c，也就是a,b的区间范围是[0,sqrt(c)]
+3 双指针i,j分别指向区间两端，如他们的平方和偏大，j--；如平方和偏小，i++。直到找到这两个数字
+4 循环终止条件j&gt;i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定一个非负整数 c ，你要判断是否存在两个整数 a 和 b，使得 a2 + b2 = c。 
+输入: 5
+输出: True
+解释: 1 * 1 + 2 * 2 = 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>双指针
+逼近</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(sqrt(n))，n是数字值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2262,10 +2285,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E584FD4-BA79-F944-99BC-B54BFFE20F3C}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2375,6 +2398,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:11" ht="154">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>633</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
two sum improve   with linkedlist
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEED474-9AD9-B442-A50F-2741AA0C1060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98F769C-EF0E-1249-B96C-C2B5A9EA15F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" activeTab="3" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="13720" yWindow="5220" windowWidth="21600" windowHeight="15500" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="138">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -923,6 +923,32 @@
   </si>
   <si>
     <t>O(sqrt(n))，n是数字值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给出两个 非空 的链表用来表示两个非负的整数。其中，它们各自的位数是按照 逆序 的方式存储的，
+ 并且它们的每个节点只能存储 一位 数字。
+ 如果，我们将这两个数相加起来，则会返回一个新的链表来表示它们的和。 
+ 您可以假设除了数字 0 之外，这两个数都不会以 0 开头。 
+ 输入：(2 -&gt; 4 -&gt; 3) + (5 -&gt; 6 -&gt; 4)
+输出：7 -&gt; 0 -&gt; 8
+原因：342 + 465 = 807</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 分别获取两个链表的头节点
+2 循环开始，循环结束条件是两个链表同时到达尾部
+3 获取两个节点的值，累加两个节点值(注意两个链表的指针也要前进)以及进位作为新的节点，保留进位，
+4 如果链表长度不等，只累加有值
+5 新的节点加入链表头部
+6 判断进位是否是1，如果是1，还需要继续将1加入和链表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进位
+solder
+链表插入
+链表迭代</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1361,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1851,6 +1877,29 @@
       </c>
       <c r="G19" s="1" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="320">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2287,8 +2336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E584FD4-BA79-F944-99BC-B54BFFE20F3C}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
delete kth node  comment  with linkedlist
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0B46B9-6F9E-2842-B7E6-D334DFE6570F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEF40DD-AE5D-8F43-9069-E94CF25E2E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13720" yWindow="5220" windowWidth="21600" windowHeight="15500" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-28320" yWindow="-13220" windowWidth="24440" windowHeight="15500" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -150,13 +150,6 @@
 K是链表个数
 堆排序的时间复杂度O(N*logN)
 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 快指针fast先从solder向前走n步
-2. 判断fast为空，就停止，确保n是一个有效范围；不为空就继续向下执行程序
-3. fast没有达到尾部，fast与slow指针同时向前走一 步，slow走第一步时是从solder走的
-4. fast到达链表尾部(非空节点)，slow就指向倒数第n个节点</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -953,6 +946,16 @@
   </si>
   <si>
     <t>O(max(M,N)),M,N是两个链表的元素个数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1 创建solder节点，连接原节点
+2 设置同侧快慢指针，fast，slow
+3 从solder节点开始，fast走n步后，slow开始走
+4 循环终止条件是fast指针到达链表尾部
+5 slow是目标节点的前一个节点
+6 执行删除操作
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1393,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1474,7 +1477,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>23</v>
+        <v>138</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>3</v>
@@ -1525,7 +1528,7 @@
         <v>61</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -1555,10 +1558,10 @@
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>9</v>
@@ -1579,13 +1582,13 @@
         <v>206</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>9</v>
@@ -1606,13 +1609,13 @@
         <v>92</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>9</v>
@@ -1633,13 +1636,13 @@
         <v>86</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>9</v>
@@ -1660,16 +1663,16 @@
         <v>141</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>5</v>
@@ -1687,13 +1690,13 @@
         <v>142</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>5</v>
@@ -1707,16 +1710,16 @@
         <v>143</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>5</v>
@@ -1730,16 +1733,16 @@
         <v>160</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>5</v>
@@ -1753,13 +1756,13 @@
         <v>203</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
@@ -1776,13 +1779,13 @@
         <v>234</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
@@ -1799,13 +1802,13 @@
         <v>237</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>5</v>
@@ -1822,13 +1825,13 @@
         <v>328</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>9</v>
@@ -1845,16 +1848,16 @@
         <v>445</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>5</v>
@@ -1868,19 +1871,19 @@
         <v>1171</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="320">
@@ -1891,19 +1894,19 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1966,13 +1969,13 @@
         <v>136</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>9</v>
@@ -1989,19 +1992,19 @@
         <v>187</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="220">
@@ -2012,19 +2015,19 @@
         <v>202</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="154">
@@ -2035,19 +2038,19 @@
         <v>347</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="154">
@@ -2058,19 +2061,19 @@
         <v>350</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="66">
@@ -2081,19 +2084,19 @@
         <v>387</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="110">
@@ -2104,19 +2107,19 @@
         <v>389</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2129,19 +2132,19 @@
         <v>451</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -2154,19 +2157,19 @@
         <v>500</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="E10" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" s="4"/>
     </row>
@@ -2178,13 +2181,13 @@
         <v>692</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -2198,13 +2201,13 @@
         <v>1160</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -2269,19 +2272,19 @@
         <v>509</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="G2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="198">
@@ -2292,19 +2295,19 @@
         <v>300</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="308">
@@ -2315,19 +2318,19 @@
         <v>674</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2390,16 +2393,16 @@
         <v>168</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>5</v>
@@ -2410,19 +2413,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>127</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>5</v>
@@ -2436,16 +2439,16 @@
         <v>263</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>129</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>5</v>
@@ -2459,16 +2462,16 @@
         <v>633</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
merge k   with linkedlist
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEF40DD-AE5D-8F43-9069-E94CF25E2E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B0986B-D912-CA47-941F-CB98B0F93383}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28320" yWindow="-13220" windowWidth="24440" windowHeight="15500" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -128,14 +128,6 @@
   </si>
   <si>
     <t>合并 k 个排序链表，返回合并后的排序链表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 建立最小堆
-2. 将各链表的头节点加入最小堆
-3. 取堆顶元素加入新的链表
-4. 堆顶元素所在的链表的下一个节点放入堆中
-5. 堆中没有元素，说明合并完成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -956,6 +948,14 @@
 5 slow是目标节点的前一个节点
 6 执行删除操作
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 建立最小堆，创建solder以及cur指针
+2. 将各链表的头节点加入最小堆
+3. 取堆顶元素加入新的链表
+4. 堆顶元素所在的链表的下一个节点放入堆中
+5. 堆中没有元素，说明合并完成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1397,7 +1397,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1450,13 +1450,13 @@
         <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>1</v>
@@ -1477,7 +1477,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>3</v>
@@ -1528,7 +1528,7 @@
         <v>61</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -1558,10 +1558,10 @@
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>9</v>
@@ -1582,13 +1582,13 @@
         <v>206</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>9</v>
@@ -1609,13 +1609,13 @@
         <v>92</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>9</v>
@@ -1636,13 +1636,13 @@
         <v>86</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>9</v>
@@ -1663,16 +1663,16 @@
         <v>141</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>5</v>
@@ -1690,13 +1690,13 @@
         <v>142</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>5</v>
@@ -1710,16 +1710,16 @@
         <v>143</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>5</v>
@@ -1733,16 +1733,16 @@
         <v>160</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>5</v>
@@ -1756,13 +1756,13 @@
         <v>203</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
@@ -1779,13 +1779,13 @@
         <v>234</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
@@ -1802,13 +1802,13 @@
         <v>237</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>5</v>
@@ -1825,13 +1825,13 @@
         <v>328</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>9</v>
@@ -1848,16 +1848,16 @@
         <v>445</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>5</v>
@@ -1871,19 +1871,19 @@
         <v>1171</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="320">
@@ -1894,19 +1894,19 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1969,13 +1969,13 @@
         <v>136</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>9</v>
@@ -1992,19 +1992,19 @@
         <v>187</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="220">
@@ -2015,19 +2015,19 @@
         <v>202</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="154">
@@ -2038,19 +2038,19 @@
         <v>347</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="154">
@@ -2061,19 +2061,19 @@
         <v>350</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="66">
@@ -2084,19 +2084,19 @@
         <v>387</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="110">
@@ -2107,19 +2107,19 @@
         <v>389</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2132,19 +2132,19 @@
         <v>451</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -2157,19 +2157,19 @@
         <v>500</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="E10" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H10" s="4"/>
     </row>
@@ -2181,13 +2181,13 @@
         <v>692</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -2201,13 +2201,13 @@
         <v>1160</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -2272,19 +2272,19 @@
         <v>509</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>110</v>
-      </c>
       <c r="G2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="198">
@@ -2295,19 +2295,19 @@
         <v>300</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="308">
@@ -2318,19 +2318,19 @@
         <v>674</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2393,16 +2393,16 @@
         <v>168</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>122</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>5</v>
@@ -2413,19 +2413,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>5</v>
@@ -2439,16 +2439,16 @@
         <v>263</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>128</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>5</v>
@@ -2462,16 +2462,16 @@
         <v>633</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>133</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
delete duplicate 2  with linkedlist
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B0986B-D912-CA47-941F-CB98B0F93383}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BED3589-3F02-5942-BDB5-8AE411016667}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28320" yWindow="-13220" windowWidth="24440" windowHeight="15500" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="15020" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="142">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -956,6 +956,35 @@
 3. 取堆顶元素加入新的链表
 4. 堆顶元素所在的链表的下一个节点放入堆中
 5. 堆中没有元素，说明合并完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">给定一个排序链表，删除所有含有重复数字的节点，只保留原始链表中 没有重复出现 的数字。 
+ 示例 1: 
+ 输入: 1-&gt;2-&gt;3-&gt;3-&gt;4-&gt;4-&gt;5
+输出: 1-&gt;2-&gt;5
+ 示例 2: 
+ 输入: 1-&gt;1-&gt;1-&gt;2-&gt;3
+输出: 2-&gt;3 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 创建solder节点，便于处理头节点重复的情况
+2 cur指针从solder开始，
+3 cur的next节点与next.next节点的值对比
+     如果不相等，就迭代cur=cur.next
+     如果相等，此时cur在相等节点之前，tmp指针作为重复节点的第一个元素迭代
+     tmp节点与tmp.next节点是否相等
+            如果相等，就继续移动tmp
+            如果不想等，cur指向tmp的下一个节点【这个节点就是重复节点链后的第一个节点】
+     循环条件是tmp的值是否与tmp.next的值相等
+4 循环结束条件是cur的next节点与next.next节点不为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">双指针
+快慢指针
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1394,18 +1423,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="4.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36" style="1" customWidth="1"/>
-    <col min="4" max="4" width="52.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="75.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.83203125" style="1" customWidth="1"/>
@@ -1907,6 +1936,23 @@
       </c>
       <c r="G20" s="1" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="240">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>82</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete duplicate 1  with linkedlist
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BED3589-3F02-5942-BDB5-8AE411016667}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C213652-65D7-594E-9970-9F08F98F6AD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="15020" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -146,14 +146,6 @@
   </si>
   <si>
     <t>给定一个链表，旋转链表，将链表每个节点向右移动 k 个位置，其中 k 是非负数。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 从solder开始遍历其后面的两个节点
-2 如果fast不为空
-3 如果fast与slow相等，共同向前走一步
-4 如果不相等，fast向前走一步，slow指向fast
-5 如果fast为空，返回solder.next</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -985,6 +977,18 @@
     <t xml:space="preserve">双指针
 快慢指针
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 参考去除重复节点，不保留重复节点
+1 创建solder节点
+2 cur节点从solder节点开始，cur.next与cur.next.next节点是否相等
+3 如果不相等，cur指针继续前进
+4 如果相等，tmp指针指向重复节点第一个节点，向前移动。判断tmp节点是否与tmp.next
+       如果相等，tmp指针向前移动
+       如果不相等，cur指向tmp节点，cur指针也要前进。实际操作是保留的重复节点的最后一个节点
+       循环结束条件是tmp.next不是null
+5 循环结束条件是cur.next以及cur.next.next不是null</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1425,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1479,7 +1483,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>20</v>
@@ -1506,7 +1510,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>3</v>
@@ -1522,7 +1526,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="154">
+    <row r="4" spans="1:11" ht="88">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1549,7 +1553,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="198">
+    <row r="5" spans="1:11" ht="154">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1576,7 +1580,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="110">
+    <row r="6" spans="1:11" ht="242">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1587,10 +1591,10 @@
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>9</v>
@@ -1603,7 +1607,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="176">
+    <row r="7" spans="1:11" ht="132">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1611,13 +1615,13 @@
         <v>206</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>9</v>
@@ -1630,7 +1634,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="308">
+    <row r="8" spans="1:11" ht="176">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1638,13 +1642,13 @@
         <v>92</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>9</v>
@@ -1657,7 +1661,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="120">
+    <row r="9" spans="1:11" ht="100">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1665,13 +1669,13 @@
         <v>86</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>9</v>
@@ -1692,16 +1696,16 @@
         <v>141</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>5</v>
@@ -1711,7 +1715,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="180">
+    <row r="11" spans="1:11" ht="160">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1719,19 +1723,19 @@
         <v>142</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="120">
+    <row r="12" spans="1:11" ht="100">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1739,22 +1743,22 @@
         <v>143</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="220">
+    <row r="13" spans="1:11" ht="160">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1762,16 +1766,16 @@
         <v>160</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>5</v>
@@ -1785,13 +1789,13 @@
         <v>203</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
@@ -1800,7 +1804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="200">
+    <row r="15" spans="1:11" ht="140">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1808,13 +1812,13 @@
         <v>234</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
@@ -1831,13 +1835,13 @@
         <v>237</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>5</v>
@@ -1854,13 +1858,13 @@
         <v>328</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>9</v>
@@ -1869,7 +1873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="120">
+    <row r="18" spans="1:7" ht="100">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1877,22 +1881,22 @@
         <v>445</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="200">
+    <row r="19" spans="1:7" ht="140">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1900,22 +1904,22 @@
         <v>1171</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="320">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="280">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1923,19 +1927,19 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="240">
@@ -1946,13 +1950,13 @@
         <v>82</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2015,13 +2019,13 @@
         <v>136</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>9</v>
@@ -2038,19 +2042,19 @@
         <v>187</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="220">
@@ -2061,19 +2065,19 @@
         <v>202</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="154">
@@ -2084,19 +2088,19 @@
         <v>347</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="154">
@@ -2107,19 +2111,19 @@
         <v>350</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="66">
@@ -2130,19 +2134,19 @@
         <v>387</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="110">
@@ -2153,19 +2157,19 @@
         <v>389</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2178,19 +2182,19 @@
         <v>451</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -2203,19 +2207,19 @@
         <v>500</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="E10" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H10" s="4"/>
     </row>
@@ -2227,13 +2231,13 @@
         <v>692</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -2247,13 +2251,13 @@
         <v>1160</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -2318,19 +2322,19 @@
         <v>509</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="G2" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="198">
@@ -2341,19 +2345,19 @@
         <v>300</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="308">
@@ -2364,19 +2368,19 @@
         <v>674</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2439,16 +2443,16 @@
         <v>168</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>5</v>
@@ -2459,19 +2463,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>125</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>5</v>
@@ -2485,16 +2489,16 @@
         <v>263</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>127</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>5</v>
@@ -2508,16 +2512,16 @@
         <v>633</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
partition  comment  with linkedlist
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C213652-65D7-594E-9970-9F08F98F6AD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880A88FF-A200-C04A-8B41-C920F486999C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="15020" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -194,76 +194,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>给定一个链表和一个特定值</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF808080"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF808080"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t>，对链表进行分隔，使得所有小于</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF808080"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> x </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF808080"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t>的节点都在大于或等于</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF808080"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> x </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF808080"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t>的节点之前</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>两个指针
 链表插入/删除</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 创建小指针min，大指针max
-2 小指针连接小于目标值的节点，大指针连接大于等于目标值的节点
-3大指针的next要赋值为null，例如1-4-3-2-5-2
-4 小指针的next指向大指针链表的头部
-5 返回小指针头部</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -989,6 +921,77 @@
        如果不相等，cur指向tmp节点，cur指针也要前进。实际操作是保留的重复节点的最后一个节点
        循环结束条件是tmp.next不是null
 5 循环结束条件是cur.next以及cur.next.next不是null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 需要创建两个链表，minSolder/minCur，maxSolder/maxCur
+2 迭代原链表，与给定值比较，插入到相关的链表
+3 迭代条件是原链表到达尾部
+4 min链表要指向max链表的头部，因此min链表尾节点不需特殊处理
+     但是原链表迭代完成，max链表有可能会指向别的元素，例如1-4-7-2-8-5，4
+     这就需要max链表的尾节点要指向null
+4 minCur指向maxSolder.next
+5 返回minSolder.next</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>给定一个链表和一个特定值</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF808080"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF808080"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>，对链表进行分隔，使得所有小于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF808080"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> x </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF808080"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>的节点都在大于或等于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF808080"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> x </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF808080"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>的节点之前</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1034,18 +1037,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF808080"/>
-      <name val="Monaco"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF808080"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1064,6 +1055,18 @@
       <name val="微软雅黑"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF808080"/>
+      <name val="Monaco"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1107,10 +1110,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1429,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1483,7 +1486,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>20</v>
@@ -1510,7 +1513,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>3</v>
@@ -1591,7 +1594,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>23</v>
@@ -1661,21 +1664,21 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="100">
+    <row r="9" spans="1:11" ht="180">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2">
         <v>86</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>9</v>
@@ -1696,16 +1699,16 @@
         <v>141</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>5</v>
@@ -1723,13 +1726,13 @@
         <v>142</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>5</v>
@@ -1743,16 +1746,16 @@
         <v>143</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>5</v>
@@ -1766,16 +1769,16 @@
         <v>160</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>5</v>
@@ -1789,13 +1792,13 @@
         <v>203</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
@@ -1812,13 +1815,13 @@
         <v>234</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
@@ -1835,13 +1838,13 @@
         <v>237</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>5</v>
@@ -1858,13 +1861,13 @@
         <v>328</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>9</v>
@@ -1881,16 +1884,16 @@
         <v>445</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>5</v>
@@ -1904,19 +1907,19 @@
         <v>1171</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="280">
@@ -1927,19 +1930,19 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="240">
@@ -1950,13 +1953,13 @@
         <v>82</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2019,13 +2022,13 @@
         <v>136</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>9</v>
@@ -2042,19 +2045,19 @@
         <v>187</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="220">
@@ -2065,19 +2068,19 @@
         <v>202</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="154">
@@ -2088,19 +2091,19 @@
         <v>347</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="F5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="154">
@@ -2111,19 +2114,19 @@
         <v>350</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="F6" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="66">
@@ -2134,19 +2137,19 @@
         <v>387</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="110">
@@ -2157,19 +2160,19 @@
         <v>389</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2182,19 +2185,19 @@
         <v>451</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -2207,19 +2210,19 @@
         <v>500</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H10" s="4"/>
     </row>
@@ -2231,13 +2234,13 @@
         <v>692</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -2251,13 +2254,13 @@
         <v>1160</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -2322,19 +2325,19 @@
         <v>509</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="G2" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="198">
@@ -2345,19 +2348,19 @@
         <v>300</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>113</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="308">
@@ -2368,19 +2371,19 @@
         <v>674</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2443,16 +2446,16 @@
         <v>168</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>5</v>
@@ -2463,19 +2466,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="D3" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>5</v>
@@ -2489,16 +2492,16 @@
         <v>263</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>127</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>5</v>
@@ -2512,16 +2515,16 @@
         <v>633</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
cycle intersection comment  with linkedlist
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CD0EDD-61ED-E74A-A346-FAD02D6668B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631F9A45-028A-3741-BD60-AD530919D67B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="15020" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-27020" yWindow="-8540" windowWidth="26880" windowHeight="15020" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -223,15 +223,6 @@
   </si>
   <si>
     <t>给定一个链表，返回链表开始入环的第一个节点。 如果链表无环，则返回 null</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 快慢指针同时指向链表头节点
-2 快指针以及后续指针不为空
-3 快指针走两步，慢指针走一步
-3 快慢指针对应的节点是否相等，如果相等就说明有环，进一步验证环的入口（有环就一定有入口）
-，快节点从头开始走，慢节点继续前进，步长均为1，当slow==fast，说明入口到了
-4 如果没有找到或者快节点为空，就说明没有环，返回null</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1017,6 +1008,19 @@
     <t>快慢指针
 相遇
 链表尾部节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1 快慢指针fast，slow从链表头部开始
+2 fast每次走两步；slow每次走一步
+3 如果fast==slow说明有环
+4 循环结束条件fast或者fast.next为空
+5 循环结束，需要判断一下是否有环
+     如果没有环(条件是fast或者fast.next是null)就返回null
+     如果有环，就将fast指针指向链表头节点，slow与fast迭代向前走一步
+     循环结束条件是fast==slow
+6. 两个指针相遇处，就是链表的入口</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1457,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1511,7 +1515,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>20</v>
@@ -1538,7 +1542,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>3</v>
@@ -1619,7 +1623,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>23</v>
@@ -1697,10 +1701,10 @@
         <v>86</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>30</v>
@@ -1743,7 +1747,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="160">
+    <row r="11" spans="1:11" ht="200">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1754,7 +1758,7 @@
         <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>144</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>33</v>
@@ -1771,16 +1775,16 @@
         <v>143</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>5</v>
@@ -1794,16 +1798,16 @@
         <v>160</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>5</v>
@@ -1817,13 +1821,13 @@
         <v>203</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
@@ -1840,13 +1844,13 @@
         <v>234</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
@@ -1863,13 +1867,13 @@
         <v>237</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>5</v>
@@ -1886,13 +1890,13 @@
         <v>328</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>9</v>
@@ -1909,16 +1913,16 @@
         <v>445</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>5</v>
@@ -1932,19 +1936,19 @@
         <v>1171</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="280">
@@ -1955,19 +1959,19 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="240">
@@ -1978,13 +1982,13 @@
         <v>82</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="240">
@@ -1995,13 +1999,13 @@
         <v>14</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -2070,13 +2074,13 @@
         <v>136</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>9</v>
@@ -2093,19 +2097,19 @@
         <v>187</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="220">
@@ -2116,19 +2120,19 @@
         <v>202</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="154">
@@ -2139,19 +2143,19 @@
         <v>347</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="154">
@@ -2162,19 +2166,19 @@
         <v>350</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="66">
@@ -2185,19 +2189,19 @@
         <v>387</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="110">
@@ -2208,19 +2212,19 @@
         <v>389</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2233,19 +2237,19 @@
         <v>451</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -2258,19 +2262,19 @@
         <v>500</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="E10" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H10" s="4"/>
     </row>
@@ -2282,13 +2286,13 @@
         <v>692</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -2302,13 +2306,13 @@
         <v>1160</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -2373,19 +2377,19 @@
         <v>509</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="G2" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="198">
@@ -2396,19 +2400,19 @@
         <v>300</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="308">
@@ -2419,19 +2423,19 @@
         <v>674</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>113</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2494,16 +2498,16 @@
         <v>168</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>5</v>
@@ -2514,19 +2518,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>122</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>5</v>
@@ -2540,16 +2544,16 @@
         <v>263</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>5</v>
@@ -2563,16 +2567,16 @@
         <v>633</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
remove zero sum with linkedlist
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A186F1-6DD7-054A-9134-6C12DD4B465A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4810ACA9-B43A-A142-B061-C34C01D88210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="15040" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -348,14 +348,6 @@
     <t>栈
 链表反转
 链表添加</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>solder方便处理1-2--3
-1 使用map，key是当前节点以及之前节点的累加和，value是当前节点对象
-2 迭代节点，cur对应的节点和存在多次，说明这中间是有连续元素和为0的节点，即1-2-3-4,&lt;0,0&gt;&lt;1,1&gt;&lt;3,2&gt;&lt;6,3&gt;&lt;3,-3&gt;&lt;7,4&gt;
-3 找到这个节点cur1，将cur.next=cur1.next
-4 如果没有连续节点和是0，在map中也能找到一次累加和，执行cur.next=cur1.next，也是一样的，因为cur=cur1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1150,6 +1142,14 @@
       即1-2-3-4-5-6-7-8，5是中间节点，计算是从6开始
       即1-2-3-4-5-6-7-8-9，6是中间节点，计算是从7开始</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>solder方便处理1-2--3
+1 使用map，key是当前节点以及之前节点的累加和，value是当前节点对象
+2 迭代节点，cur对应的节点和存在多次，说明这中间是有连续元素和为0的节点，即1-2-3-4,&lt;0,0&gt;&lt;1,1&gt;&lt;3,2&gt;&lt;6,3&gt;&lt;3,-3&gt;&lt;7,4&gt;
+3 找到这个节点cur1，将cur.next=cur1.next，直接处理的最外侧，嵌套的不需要处理，例如1-2-3--3--2-4-5--5-6
+4 如果没有连续节点和是0，在map中也能找到一次累加和，执行cur.next=cur1.next，也是一样的，因为cur=cur1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1597,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1651,7 +1651,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>20</v>
@@ -1678,7 +1678,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>3</v>
@@ -1759,7 +1759,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>23</v>
@@ -1837,10 +1837,10 @@
         <v>86</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>30</v>
@@ -1894,7 +1894,7 @@
         <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>33</v>
@@ -1914,7 +1914,7 @@
         <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>37</v>
@@ -2064,7 +2064,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="140">
+    <row r="19" spans="1:7" ht="160">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2072,19 +2072,19 @@
         <v>1171</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="280">
@@ -2095,19 +2095,19 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="240">
@@ -2118,13 +2118,13 @@
         <v>82</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="240">
@@ -2135,13 +2135,13 @@
         <v>14</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -2210,13 +2210,13 @@
         <v>136</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>9</v>
@@ -2233,19 +2233,19 @@
         <v>187</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="220">
@@ -2256,19 +2256,19 @@
         <v>202</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="154">
@@ -2279,19 +2279,19 @@
         <v>347</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="154">
@@ -2302,19 +2302,19 @@
         <v>350</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="66">
@@ -2325,19 +2325,19 @@
         <v>387</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="110">
@@ -2348,19 +2348,19 @@
         <v>389</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2373,19 +2373,19 @@
         <v>451</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -2398,19 +2398,19 @@
         <v>500</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="E10" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H10" s="4"/>
     </row>
@@ -2422,13 +2422,13 @@
         <v>692</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -2442,13 +2442,13 @@
         <v>1160</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -2513,19 +2513,19 @@
         <v>509</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>104</v>
-      </c>
       <c r="G2" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="198">
@@ -2536,19 +2536,19 @@
         <v>300</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="308">
@@ -2559,19 +2559,19 @@
         <v>674</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2634,16 +2634,16 @@
         <v>168</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>5</v>
@@ -2654,19 +2654,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>5</v>
@@ -2680,16 +2680,16 @@
         <v>263</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>122</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>5</v>
@@ -2703,16 +2703,16 @@
         <v>633</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
two number sum  with hashmap
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4810ACA9-B43A-A142-B061-C34C01D88210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A58062B-30FA-D042-907A-6B7B1DFDEC25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="15040" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="15040" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="148">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1150,6 +1150,24 @@
 2 迭代节点，cur对应的节点和存在多次，说明这中间是有连续元素和为0的节点，即1-2-3-4,&lt;0,0&gt;&lt;1,1&gt;&lt;3,2&gt;&lt;6,3&gt;&lt;3,-3&gt;&lt;7,4&gt;
 3 找到这个节点cur1，将cur.next=cur1.next，直接处理的最外侧，嵌套的不需要处理，例如1-2-3--3--2-4-5--5-6
 4 如果没有连续节点和是0，在map中也能找到一次累加和，执行cur.next=cur1.next，也是一样的，因为cur=cur1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">给定一个整数数组 nums 和一个目标值 target，请你在该数组中找出和为目标值的那 两个 整数，并返回他们的数组下标。 
+ 你可以假设每种输入只会对应一个答案。但是，数组中同一个元素不能使用两遍。 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 map的key存储目标值target-当前数字的差值，value存储当前位置
+2 遍历数组，当前数字是否在map中，
+       如果不存在就将target-val作为key，index作为value存入map
+        如果存在，就说明找到了这个数字。
+        返回这两个数字的下标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哈希表
+两数之和</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1597,7 +1615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507AAD-2277-8248-9E9C-02E825D54774}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -2158,10 +2176,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A17B2E-7C89-9142-AF64-850FAB88A98B}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2452,6 +2470,29 @@
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" ht="176">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
number once  with hashmap
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A58062B-30FA-D042-907A-6B7B1DFDEC25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4CDDFE-B614-8042-BEAF-D94A46DF3C59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="15040" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -2176,10 +2176,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A17B2E-7C89-9142-AF64-850FAB88A98B}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2493,6 +2493,12 @@
       <c r="G13" s="4" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="14" spans="1:11" ht="21">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
duplicate 2  with hashmap
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4CDDFE-B614-8042-BEAF-D94A46DF3C59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9657A2BF-E642-1F4D-9003-BD978208F8A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="15040" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-140" yWindow="1960" windowWidth="26880" windowHeight="15040" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="151">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1168,6 +1168,31 @@
   <si>
     <t>哈希表
 两数之和</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">给定一个整数数组和一个整数 k，判断数组中是否存在两个不同的索引 i 和 j，使 nums [i] = nums [j]，并且 i 和 j 的差的 绝对值至多为 k。 
+ 示例 1:
+ 输入: nums = [1,2,3,1], k = 3
+输出: true </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哈希表
+索引</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 迭代数组，存入map，key是元素值，value是其索引值
+2 判断元素是否在map中，如果不在就加入map
+3 如果存在
+    判断其索引值差值&lt;=k，return true
+    判断其索引值差值&gt;k，将现在的index索引值保存，继续迭代
+4 迭代结束条件是遍历完数组元素
+另一方案是使用集合，基于长度是k的窗口：
+         1 判断集合中是否存在此元素，不存在就添加此元素
+         2 如果集合元素个数超过k，将最前面元素删除，始终保持集合元素个数是k
+         3 如果集合中包含此元素，就是满足需要</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2179,7 +2204,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2494,11 +2519,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="21">
+    <row r="14" spans="1:11" ht="308">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4">
+        <v>219</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
duplicate frequency  with hashmap
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9657A2BF-E642-1F4D-9003-BD978208F8A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB88286-31D4-9E41-8F39-2FA942AFEFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-140" yWindow="1960" windowWidth="26880" windowHeight="15040" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="0" yWindow="1760" windowWidth="26880" windowHeight="15040" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -2203,8 +2203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A17B2E-7C89-9142-AF64-850FAB88A98B}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
remove duplicate number  with hashmap
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB88286-31D4-9E41-8F39-2FA942AFEFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8072FE-191D-8345-996A-CD6D94B3F474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1760" windowWidth="26880" windowHeight="15040" activeTab="1" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-38140" yWindow="460" windowWidth="26880" windowHeight="15040" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
     <sheet name="哈希" sheetId="2" r:id="rId2"/>
     <sheet name="动态规划" sheetId="3" r:id="rId3"/>
     <sheet name="数学" sheetId="4" r:id="rId4"/>
+    <sheet name="数组" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="152">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1193,6 +1194,31 @@
          1 判断集合中是否存在此元素，不存在就添加此元素
          2 如果集合元素个数超过k，将最前面元素删除，始终保持集合元素个数是k
          3 如果集合中包含此元素，就是满足需要</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+给定一个排序数组，你需要在 原地 删除重复出现的元素，使得每个元素只出现一次，返回移除后数组的新长度。 
+ 不要使用额外的数组空间，你必须在 原地 修改输入数组 并在使用 O(1) 额外空间的条件下完成。
+ 示例 1:
+ 给定数组 nums = [1,1,2],
+函数应该返回新的长度 2, 并且原数组 nums 的前两个元素被修改为 1, 2。
+你不需要考虑数组中超出新长度后面的元素。
+ 示例 2:
+ 给定 nums = [0,0,1,1,1,2,2,3,3,4],
+函数应该返回新的长度 5, 并且原数组 nums 的前五个元素被修改为 0, 1, 2, 3, 4。
+你不需要考虑数组中超出新长度后面的元素。
+ 说明: 
+ 为什么返回数值是整数，但输出的答案是数组呢?
+ 请注意，输入数组是以「引用」方式传递的，这意味着在函数里修改输入数组对于调用者是可见的。 
+ 你可以想象内部操作如下:
+ // nums 是以“引用”方式传递的。也就是说，不对实参做任何拷贝
+int len = removeDuplicates(nums);
+// 在函数里修改输入数组对于调用者是可见的。
+// 根据你的函数返回的长度, 它会打印出数组中该长度范围内的所有元素。
+for (int i = 0; i &lt; len; i++) {
+    print(nums[i]);
+}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2203,7 +2229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A17B2E-7C89-9142-AF64-850FAB88A98B}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2673,8 +2699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E584FD4-BA79-F944-99BC-B54BFFE20F3C}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2811,4 +2837,67 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1220750-1EE9-8D43-BAD7-661B81A9AEFD}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" customWidth="1"/>
+    <col min="4" max="4" width="76.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="409.6">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
remove duplicate number 2   with hashmap
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E271870-1A93-834C-9236-D56693849E25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD20A835-EC6F-A44D-8999-48118B0F4F8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-20" yWindow="2740" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="157">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1236,6 +1236,44 @@
 数组元素覆盖</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>1 设置动态指针index=0，用于指向最终数组的下标。遍历数组，判断元素是否与目标元素相等
+2 如果不相等，就将nums[i]赋值给num[index++]
+3 如果相等，继续遍历，直到数组结束
+4 目标数组长度就是index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给你一个数组 nums 和一个值 val，你需要 原地 移除所有数值等于 val 的元素，并返回移除数组的新长度。 
+ 不要使用额外的数组空间，你必须仅使用 O(1) 额外空间并 原地 修改输入数组。 
+ 元素的顺序可以改变。你不需要考虑数组中超出新长度后面的元素。 
+ 示例 1:
+ 给定 nums = [3,2,2,3], val = 3,
+函数应该返回新的长度 2, 并且 nums 中的前两个元素均为 2。
+你不需要考虑数组中超出新长度后面的元素。
+ 示例 2:
+ 给定 nums = [0,1,2,2,3,0,4,2], val = 2,
+函数应该返回新的长度 5, 并且 nums 中的前五个元素为 0, 1, 3, 0, 4。
+注意这五个元素可为任意顺序。
+你不需要考虑数组中超出新长度后面的元素。
+ 说明:
+ 为什么返回数值是整数，但输出的答案是数组呢? 
+ 请注意，输入数组是以「引用」方式传递的，这意味着在函数里修改输入数组对于调用者是可见。 
+ 你可以想象内部操作如下: 
+ // nums 是以“引用”方式传递的。也就是说，不对实参作任何拷贝
+int len = removeElement(nums, val);
+// 在函数里修改输入数组对于调用者是可见的。
+// 根据你的函数返回的长度, 它会打印出数组中 该长度范围内 的所有元素。
+for (int i = 0; i &lt; len; i++) {
+    print(nums[i]);
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>覆盖
+额外指针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1340,7 +1378,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1364,6 +1402,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2858,8 +2899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1220750-1EE9-8D43-BAD7-661B81A9AEFD}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2919,12 +2960,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="409.6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>27</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
location with bs  with hashmap
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD20A835-EC6F-A44D-8999-48118B0F4F8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E4517F-8F20-8240-9377-7F830E06203E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="2740" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="0" yWindow="2740" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -1378,7 +1378,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1402,9 +1402,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2900,40 +2897,40 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="61.1640625" customWidth="1"/>
-    <col min="4" max="4" width="76.1640625" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="76.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2961,25 +2958,25 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="409.6">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>27</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sub array with array
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2B4EEF-5083-A143-BBF5-675577593F64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22058A9-F8E2-2840-8BCB-D554A190C862}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2740" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -1275,24 +1275,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">  设计算法
-  1 二分查找目标元素，如果找到了返回索引值
-  2 同时使用两个变量存储最近两次的中间位置mid1,mid2
-  3 没有找到就将目标值查到mid1,mid2中间位置
-  测试用例
-  1 1,3,5,7 5
-  1 1,3,5,7 1
-  1 1,3,5,7 7
-  2 1,3,5 0
-  2 1,3,5 6
-  2 1,3,5 4
-  或者归纳一下，可知返回的是low
-  1,3,5,6 7
-  1,3,5,6 0
-  1,3,5,6 4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>给定一个排序数组和一个目标值，在数组中找到目标值，并返回其索引。如果目标值不存在于数组中，返回它将会被按顺序插入的位置。 
 你可以假设数组中无重复元素。
 示例 1:
@@ -1317,6 +1299,23 @@
   </si>
   <si>
     <t>O(logN)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  设计算法
+  1 二分查找目标元素，如果找到了返回索引值
+  2 没有找到就将返回low
+  测试用例
+  1 1,3,5,7 5
+  1 1,3,5,7 1
+  1 1,3,5,7 7
+  2 1,3,5 0
+  2 1,3,5 6
+  2 1,3,5 4
+  或者归纳一下，可知返回的是low
+  1,3,5,6 7
+  1,3,5,6 0
+  1,3,5,6 4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3025,7 +3024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="374">
+    <row r="4" spans="1:7" ht="352">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -3033,16 +3032,16 @@
         <v>35</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
plus 1 code improve  with array
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C5D9DC-6A8F-B046-A24A-6E5E2B933C2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ADE6F6-ADF7-CD48-A05B-05DECB96BE00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2740" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="167">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1342,6 +1342,35 @@
     <t>动态规划
 累加
 最大值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定一个由整数组成的非空数组所表示的非负整数，在该数的基础上加一。 
+ 最高位数字存放在数组的首位， 数组中每个元素只存储单个数字。 
+ 你可以假设除了整数 0 之外，这个整数不会以零开头。 
+ 示例 1: 
+ 输入: [1,2,3]
+输出: [1,2,4]
+解释: 输入数组表示数字 123。
+ 示例 2: 
+ 输入: [4,3,2,1]
+输出: [4,3,2,2]
+解释: 输入数组表示数字 4321。
+ Related Topics 数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 迭代数组
+1 获取数值并且加一
+     如果之和等于10，说明这个原数字是9，应该将这一位变成，放心：下一次的循环会直接digits[i] = digits[i] + 1;
+     如果之和不扽与10，说明没有进位，就可以直接返回当前的结果
+2 继续迭代
+3 数组迭代完成，说明最高位还有进位，创建新数组保存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相加
+进位</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2964,10 +2993,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1220750-1EE9-8D43-BAD7-661B81A9AEFD}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -3096,6 +3125,29 @@
         <v>85</v>
       </c>
     </row>
+    <row r="6" spans="1:7" ht="409.6">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>66</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
peak code  with array
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ADE6F6-ADF7-CD48-A05B-05DECB96BE00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75C4CE9-7E2B-9F42-BA75-4172E0636C20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2740" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="170">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1371,6 +1371,39 @@
   <si>
     <t>相加
 进位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 基于二分查找思想，获取数组中间节点mid
+2 num[mid] &lt; num[mid+1] 升序，峰值在右侧，mid肯定不是峰值，low = mid+1
+3 num[mid] &gt; num[mid+1] 这部分是降序，峰值在左侧，有可能mid就是峰值，high = mid - 1
+4 不会出现相邻元素相等的情况，代码中可以处理这个情况
+5 最终可以返回low/high索引</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>峰值元素是指其值大于左右相邻值的元素。 
+ 给定一个输入数组 nums，其中 nums[i] ≠ nums[i+1]，找到峰值元素并返回其索引。 
+ 数组可能包含多个峰值，在这种情况下，返回任何一个峰值所在位置即可。 
+ 你可以假设 nums[-1] = nums[n] = -∞。 
+ 示例 1: 
+ 输入: nums = [1,2,3,1]
+输出: 2
+解释: 3 是峰值元素，你的函数应该返回其索引 2。 
+ 示例 2: 
+ 输入: nums = [1,2,1,3,5,6,4]
+输出: 1 或 5 
+解释: 你的函数可以返回索引 1，其峰值元素为 2；
+     或者返回索引 5， 其峰值元素为 6。
+ 说明: 
+ 你的解法应该是 O(logN) 时间复杂度的。 
+ Related Topics 数组 二分查找</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">二分查找
+升序/降序
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2993,10 +3026,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1220750-1EE9-8D43-BAD7-661B81A9AEFD}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -3148,6 +3181,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:7" ht="409.6">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>162</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sum target code  with array
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75C4CE9-7E2B-9F42-BA75-4172E0636C20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B8C786-CB83-1649-9557-E36A76D102D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2740" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="6900" yWindow="5080" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="173">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1404,6 +1404,33 @@
     <t xml:space="preserve">二分查找
 升序/降序
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 数组已经排序，设置前后指针low=0，high=nums.length-1
+2 计算两个指针之和是否是目标值，如果是则返回
+3 如果和大于target，说明high左移可以让和变小（数组有序），high左移
+4 如果和小于target，说明low右移可以让和变大（数组有序），low右移
+5 循环存在条件是low &lt; high
+6 返回low+1,high+1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定一个已按照升序排列 的有序数组，找到两个数使得它们相加之和等于目标数。 
+ 函数应该返回这两个下标值 index1 和 index2，其中 index1 必须小于 index2。 
+ 说明: 
+ 返回的下标值（index1 和 index2）不是从零开始的。 
+ 你可以假设每个输入只对应唯一的答案，而且你不可以重复使用相同的元素。 
+ 示例: 
+ 输入: numbers = [2, 7, 11, 15], target = 9
+输出: [1,2]
+解释: 2 与 7 之和等于目标数 9 。因此 index1 = 1, index2 = 2 。 
+ Related Topics 数组 双指针 二分查找</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>排序
+左右双指针</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3026,10 +3053,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1220750-1EE9-8D43-BAD7-661B81A9AEFD}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -3204,6 +3231,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:7" ht="374">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>167</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
majority moer denote  with array
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B8C786-CB83-1649-9557-E36A76D102D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342CD46E-6E26-7044-A585-AD2A633DA909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="5080" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="0" yWindow="2780" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="176">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1431,6 +1431,31 @@
   <si>
     <t>排序
 左右双指针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 题目要求一定存在这样一个元素；只会有一个元素是多数元素
+2 摩尔投票法https://leetcode-cn.com/problems/majority-element/solution/tu-jie-mo-er-tou-piao-fa-python-go-by-jalan/
+3 设定第一个元素num出现次数count是1
+4 如果上一个元素不同于当前元素,count--
+5 如果count=0，当前元素作为基准元素，count=1
+6 迭代结束，基准元素就是多数元素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定一个大小为 n 的数组，找到其中的多数元素。多数元素是指在数组中出现次数大于 ⌊ n/2 ⌋ 的元素。 
+ 你可以假设数组是非空的，并且给定的数组总是存在多数元素。 
+ 示例 1:
+ 输入: [3,2,3]
+输出: 3 
+ 示例 2: 
+ 输入: [2,2,1,1,1,2,2]
+输出: 2
+ Related Topics 位运算 数组 分治算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>摩尔投票法</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3053,10 +3078,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1220750-1EE9-8D43-BAD7-661B81A9AEFD}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -3254,6 +3279,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:7" ht="352">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>169</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
repeat 2 code  with array
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342CD46E-6E26-7044-A585-AD2A633DA909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC028B0-EDCE-B640-A590-164166DF80C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2780" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="-100" yWindow="460" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="179">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1456,6 +1456,31 @@
   </si>
   <si>
     <t>摩尔投票法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">给定一个整数数组和一个整数 k，判断数组中是否存在两个不同的索引 i 和 j，使得 nums [i] = nums [j]，并且 i 和 j 的差的 绝对值
+ 至多为 k。 
+ 示例 1:
+ 输入: nums = [1,2,3,1], k = 3
+输出: true 
+ 示例 2:
+ 输入: nums = [1,0,1,1], k = 1
+输出: true 
+ 示例 3:
+ 输入: nums = [1,2,3,1,2,3], k = 2
+输出: false </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 使用hash表存储数组元素以及相应的索引
+2 如果不存在，舅加入map
+2 如果元素已存在，比较两个索引是否满足条件，满足就返回，不满足需要更新元素在map中的值，处理(1,0,1,1 1)的情况
+3 迭代结束条件是元素是否已迭代完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新map</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3078,10 +3103,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1220750-1EE9-8D43-BAD7-661B81A9AEFD}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -3302,6 +3327,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="10" spans="1:7" ht="286">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>219</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
move 0 code and design   with array
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC028B0-EDCE-B640-A590-164166DF80C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1047BE0F-DFFE-CC41-9CA3-0B9419713B53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="460" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="182">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1481,6 +1481,29 @@
   </si>
   <si>
     <t>更新map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定一个数组 nums，编写一个函数将所有 0 移动到数组的末尾，同时保持非零元素的相对顺序。 
+示例:
+输入: [0,1,0,3,12]
+输出: [1,3,12,0,0] 
+ 说明:
+ 必须在原数组上操作，不能拷贝额外的数组。
+ 尽量减少操作次数。 
+ Related Topics 数组 双指针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 定义index字段，只想非0的元素
+2 如果i位置当前元素是0，则迭代继续
+3 如果i位置当前不是0，就将这个元素，移动到index的位置，并且index++
+4 迭代完成数组元素，从index位置到数组终点，填充为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>双指针
+数组覆盖</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3103,10 +3126,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1220750-1EE9-8D43-BAD7-661B81A9AEFD}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -3350,6 +3373,29 @@
         <v>85</v>
       </c>
     </row>
+    <row r="11" spans="1:7" ht="198">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>283</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
max 1  comment  with array
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1047BE0F-DFFE-CC41-9CA3-0B9419713B53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65103EF-E74E-B143-ABBF-9707A776B8A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="8060" yWindow="3280" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="185">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1504,6 +1504,32 @@
   <si>
     <t>双指针
 数组覆盖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 初始化max=0，累加变量count=0，迭代数组元素
+2 如果元素是1，就count++
+3 如果元素是0，count=0
+4 无论是否是1，取max与count的最大值赋值给max，这个办法比较耗时
+优化：只有是0的时候取max，迭代结束再次判断max
+5 迭代结束，max就是最终结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定一个二进制数组， 计算其中最大连续1的个数。 
+ 示例 1: 
+输入: [1,1,0,1,1,1]
+输出: 3
+解释: 开头的两位和最后的三位都是连续1，所以最大连续1的个数是 3.
+ 注意： 
+ 输入的数组只包含 0 和1。 
+ 输入数组的长度是正整数，且不超过 10,000。 
+ Related Topics 数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保留上次最大值
+计数器清零</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3126,10 +3152,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1220750-1EE9-8D43-BAD7-661B81A9AEFD}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -3396,6 +3422,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="12" spans="1:7" ht="286">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>485</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
avg comment  with array
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65103EF-E74E-B143-ABBF-9707A776B8A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189CCC72-ED9F-E34B-8690-E69CC34569A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8060" yWindow="3280" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
+    <workbookView xWindow="0" yWindow="2780" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
   <sheets>
     <sheet name="链表" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="188">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1530,6 +1530,30 @@
   <si>
     <t>保留上次最大值
 计数器清零</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定 n 个整数，找出平均数最大且长度为 k 的连续子数组，并输出该最大平均数。 
+ 示例 1:
+ 输入: [1,12,-5,-6,50,3], k = 4
+输出: 12.75
+解释: 最大平均数 (12-5-6+50)/4 = 51/4 = 12.75
+ 注意:
+ 1 &lt;= k &lt;= n &lt;= 30,000。
+ 所给数据范围 [-10,000，10,000]。 
+ Related Topics 数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 计算数组中k个连续数字的累加和最大
+2 向前移动一个位置，不可以将k个数字累加，此方案效率很低，可以将当前的和去头加尾，获取max
+3 注意：使用前k个数字初始化，迭代范围是[1,len - k + 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>窗口算法
+累加
+计算最大值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3152,10 +3176,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1220750-1EE9-8D43-BAD7-661B81A9AEFD}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -3445,6 +3469,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="13" spans="1:7" ht="220">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>643</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
top k word code  with array
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189CCC72-ED9F-E34B-8690-E69CC34569A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD022F5A-C2E8-CF49-8D7B-CB60EB96C546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2780" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="192">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1554,6 +1554,46 @@
     <t>窗口算法
 累加
 计算最大值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">给一非空的单词列表，返回前 k 个出现次数最多的单词。 
+ 返回的答案应该按单词出现频率由高到低排序。如果不同的单词有相同出现频率，按字母顺序排序。 
+ 示例 1： 
+输入: ["i", "love", "leetcode", "i", "love", "coding"], k = 2
+输出: ["i", "love"]
+解析: "i" 和 "love" 为出现次数最多的两个单词，均为2次。
+    注意，按字母顺序 "i" 在 "love" 之前。
+ 示例 2： 
+输入: ["the", "day", "is", "sunny", "the", "the", "the", "sunny", "is", "is"], k
+ = 4
+输出: ["the", "is", "sunny", "day"]
+解析: "the", "is", "sunny" 和 "day" 是出现次数最多的四个单词，
+    出现次数依次为 4, 3, 2 和 1 次。
+ 注意： 
+ 假定 k 总为有效值， 1 ≤ k ≤ 集合元素数。 
+ 输入的单词均由小写字母组成。 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 创建小顶堆，存放k个单词，并且小定堆支持根据字母顺序排序单词
+2 迭代数组元素，基于map统计每个单词出现的次数
+3 迭代map中的元素，保证小顶堆中没有重复元素，不是原数组的元素。将单词放入小顶堆中，限定小顶堆长度是k
+4 将元素键入小顶堆后判断是否长度=k+1，只有k+1各元素，才能堆化，并移除不满足条件的元素，而不是k个元素。
+     如果相等就移除堆顶元素，如果没有就继续添加，知道将所有元素迭代完。
+     例如小顶堆中是2，4，6。加入7之前需要先移除2，得到的4，6，7是没有问题的。
+     但是如果加入1，最终得到的是1，4，6，但是实际上应该是2，4，6。即先将1加入并堆化后，得到1，2，4，6，然后移除1得到2，4，6
+5 输出堆中的元素到list，插入到0位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小顶堆
+堆长度
+比较字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(KlogN)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3176,10 +3216,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1220750-1EE9-8D43-BAD7-661B81A9AEFD}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -3492,6 +3532,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="14" spans="1:7" ht="409.6">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4">
+        <v>692</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
pivot code  with array
</commit_message>
<xml_diff>
--- a/src/main/java/summary/题目清单.xlsx
+++ b/src/main/java/summary/题目清单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob/code/javaProject/DataStructure/src/main/java/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD022F5A-C2E8-CF49-8D7B-CB60EB96C546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C5E820-B493-4E4E-B369-9D93FAD436B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2780" windowWidth="26880" windowHeight="14020" activeTab="4" xr2:uid="{20C558B1-3B3D-3E4A-B5AE-917A5D5001B4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="195">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1594,6 +1594,43 @@
   </si>
   <si>
     <t>O(KlogN)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定一个整数类型的数组 nums，请编写一个能够返回数组“中心索引”的方法。 
+ 我们是这样定义数组中心索引的：数组中心索引的左侧所有元素相加的和等于右侧所有元素相加的和。 
+ 如果数组不存在中心索引，那么我们应该返回 -1。如果数组有多个中心索引，那么我们应该返回最靠近左边的那一个。 
+ 示例 1:
+输入:
+nums = [1, 7, 3, 6, 5, 6]
+输出: 3
+解释: 
+索引3 (nums[3] = 6) 的左侧数之和(1 + 7 + 3 = 11)，与右侧数之和(5 + 6 = 11)相等。
+同时, 3 也是第一个符合要求的中心索引。
+ 示例 2:
+输入:
+nums = [1, 2, 3]
+输出: -1
+解释: 
+数组中不存在满足此条件的中心索引。 
+ 说明: 
+ nums 的长度范围为 [0, 10000]。
+ 任何一个 nums[i] 将会是一个范围在 [-1000, 1000]的整数。 
+ Related Topics 数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 根据数学公式推导：left + mid + right = sum =&gt; 2 * left + mid = sum
+2 计算数组的元素之和
+2 迭代数组，结束条件是找到这个中间值或者数组元素迭代完成
+3 定义left=nums[0]，用于mid左边数据的累加。
+4 从第i(i=0)个位置开始，2*left + num[i]是否等于sum,left = left + num[i]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>累加
+连续数列之和
+公示计算</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3216,10 +3253,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1220750-1EE9-8D43-BAD7-661B81A9AEFD}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -3555,6 +3592,29 @@
         <v>85</v>
       </c>
     </row>
+    <row r="15" spans="1:7" ht="409.6">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <v>724</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>